<commit_message>
SO Test cases updated in Automation org
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SOAPI.xlsx
+++ b/templates/AutomationOrg/SOAPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A9332D-1A27-484F-95C7-73B891F097E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3955BB77-B1BE-42A3-96A1-8B3F48D5E04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="807" activeTab="8" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
+    <workbookView xWindow="60" yWindow="2625" windowWidth="20430" windowHeight="7875" tabRatio="807" activeTab="8" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Header" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="57">
   <si>
     <t>API Mode</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>a3A5f000000xO8e</t>
+  </si>
+  <si>
+    <t>a6B5f000000PqATEA0</t>
+  </si>
+  <si>
+    <t>https://automationtesting2--rstk.visualforce.com/apex/soline?id=</t>
+  </si>
+  <si>
+    <t>SOLine_DeletePage</t>
   </si>
 </sst>
 </file>
@@ -580,7 +589,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -648,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D2912C-F36A-4ECF-8EDC-A40A837A9A1D}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +755,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
         <v>44</v>
@@ -755,7 +764,7 @@
         <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="M2" t="s">
         <v>47</v>
@@ -781,7 +790,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +831,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1084,10 +1093,114 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E2E4B4-F8F1-4C6E-9FE2-5A2D837A3692}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B561E7FA-B068-4DB0-B188-DC7ABD95D262}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1257,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1179,12 +1292,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B561E7FA-B068-4DB0-B188-DC7ABD95D262}">
-  <dimension ref="A1:K2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01441D4A-905D-429D-878C-59DD43158E54}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1314,7 @@
     <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1235,13 +1348,16 @@
       <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1270,102 +1386,8 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01441D4A-905D-429D-878C-59DD43158E54}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
+      <c r="L2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1377,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC22D3-7105-47EB-9F93-CBB5CCC1A1D8}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1481,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1492,7 +1514,7 @@
         <v>31</v>
       </c>
       <c r="M2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>53</v>
@@ -1516,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0427A9-21DA-4804-AC3D-33AA86AB41F7}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1616,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1603,7 +1625,7 @@
         <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>46</v>
@@ -1627,7 +1649,7 @@
         <v>43</v>
       </c>
       <c r="M2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>4</v>

</xml_diff>

<commit_message>
Updated SO Header creation based on Order Number, Created Test Plans, Added TC for Credit Hold, SO fulfillment through API
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SOAPI.xlsx
+++ b/templates/AutomationOrg/SOAPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3955BB77-B1BE-42A3-96A1-8B3F48D5E04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77650979-3173-42AE-B678-64D094AA2767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="2625" windowWidth="20430" windowHeight="7875" tabRatio="807" activeTab="8" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
+    <workbookView xWindow="20505" yWindow="60" windowWidth="28710" windowHeight="10890" tabRatio="807" activeTab="8" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Header" sheetId="1" r:id="rId1"/>
@@ -188,21 +188,6 @@
     <t>a5L5f000000gcpuEAA</t>
   </si>
   <si>
-    <t>a7S5f000000kRvX</t>
-  </si>
-  <si>
-    <t>a7S5f000000kRvc</t>
-  </si>
-  <si>
-    <t>a7S5f000000kRvh</t>
-  </si>
-  <si>
-    <t>a7S5f000000kRvm</t>
-  </si>
-  <si>
-    <t>a7S5f000000kRvr</t>
-  </si>
-  <si>
     <t>a3A5f000000xO8e</t>
   </si>
   <si>
@@ -213,6 +198,21 @@
   </si>
   <si>
     <t>SOLine_DeletePage</t>
+  </si>
+  <si>
+    <t>a7S5f000000kWRR</t>
+  </si>
+  <si>
+    <t>a7S5f000000kWRW</t>
+  </si>
+  <si>
+    <t>a7S5f000000kWRb</t>
+  </si>
+  <si>
+    <t>a7S5f000000kWRg</t>
+  </si>
+  <si>
+    <t>a7S5f000000kWRl</t>
   </si>
 </sst>
 </file>
@@ -764,7 +764,7 @@
         <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="M2" t="s">
         <v>47</v>
@@ -859,7 +859,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +931,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -966,7 +966,7 @@
         <v>46</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -1001,7 +1001,7 @@
         <v>46</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -1036,7 +1036,7 @@
         <v>46</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -1071,7 +1071,7 @@
         <v>46</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -1088,6 +1088,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1096,7 +1097,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1172,7 +1173,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1187,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1200,7 +1201,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1273,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1297,7 +1298,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1350,7 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1372,7 +1373,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1387,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1401,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1497,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1517,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="O2">
         <v>4</v>
@@ -1538,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0427A9-21DA-4804-AC3D-33AA86AB41F7}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,13 +1626,13 @@
         <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>2</v>

</xml_diff>

<commit_message>
Update asynchronous processing flag form True to False for some SOAPI TCs
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SOAPI.xlsx
+++ b/templates/AutomationOrg/SOAPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\git\rsqasampleproj\templates\AutomationOrg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77650979-3173-42AE-B678-64D094AA2767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ACA57C-13A0-4B39-8E2D-E1E12D3EF646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20505" yWindow="60" windowWidth="28710" windowHeight="10890" tabRatio="807" activeTab="8" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
+    <workbookView xWindow="25770" yWindow="2745" windowWidth="15375" windowHeight="7875" tabRatio="807" firstSheet="2" activeTab="7" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Header" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D2912C-F36A-4ECF-8EDC-A40A837A9A1D}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1096,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E2E4B4-F8F1-4C6E-9FE2-5A2D837A3692}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1298,7 +1298,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC22D3-7105-47EB-9F93-CBB5CCC1A1D8}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1539,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0427A9-21DA-4804-AC3D-33AA86AB41F7}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>